<commit_message>
Committing System_Setup3 including CRUD testcases of Feature category and VAT Class.
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/CRUD-Create Terms Code.xlsx
+++ b/templates/AutomationOrg/CRUD-Create Terms Code.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkakade\Provar\Workspace\System Setup\templates\AutomationOrg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C50C4FD-796C-4650-83BD-0B054E6E970B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C2CDB6-CE37-48E6-9FF5-C289FE15CEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0F3D348F-F58E-4F61-9FF8-3FC32BD9E731}"/>
+    <workbookView xWindow="876" yWindow="3336" windowWidth="15912" windowHeight="8964" activeTab="1" xr2:uid="{0F3D348F-F58E-4F61-9FF8-3FC32BD9E731}"/>
   </bookViews>
   <sheets>
     <sheet name="Create_Create Terms Code" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Code</t>
   </si>
@@ -101,7 +101,40 @@
     <t>TermsCode2</t>
   </si>
   <si>
-    <t>PK Terms Code 1</t>
+    <t>PK Terms Code Update</t>
+  </si>
+  <si>
+    <t>DueinDays</t>
+  </si>
+  <si>
+    <t>ReceivablesDiscountBaseDateMethod</t>
+  </si>
+  <si>
+    <t>DiscountDaysfromBaseDate</t>
+  </si>
+  <si>
+    <t>DiscountPercentage</t>
+  </si>
+  <si>
+    <t>FinanceChargeBaseDateMethod</t>
+  </si>
+  <si>
+    <t>FinanceChargeDaysfromBaseDate</t>
+  </si>
+  <si>
+    <t>FinanceChargePercentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PayablesDiscountBaseDateMethod	</t>
+  </si>
+  <si>
+    <t>IncTaxandFreightinDiscountableAmt</t>
+  </si>
+  <si>
+    <t>PK Terms Code Update1</t>
+  </si>
+  <si>
+    <t>PK Terms Code Update2</t>
   </si>
 </sst>
 </file>
@@ -455,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71E560E6-2173-495C-93A4-EFA1E9CB3BB2}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection sqref="A1:K4"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,31 +515,31 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -624,12 +657,14 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -707,7 +742,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -742,7 +777,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="C4">
         <v>10</v>

</xml_diff>